<commit_message>
Updated parts list, added a port mapping cheat sheet for the ATmega32U4
</commit_message>
<xml_diff>
--- a/Parts_List.xlsx
+++ b/Parts_List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3320" yWindow="0" windowWidth="25600" windowHeight="14080" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
   <si>
     <t>Item No.</t>
   </si>
@@ -156,13 +156,22 @@
     <t>For gain control</t>
   </si>
   <si>
-    <t>For possible microphone connection</t>
-  </si>
-  <si>
     <t>For audio in</t>
   </si>
   <si>
     <t>For programming the controller</t>
+  </si>
+  <si>
+    <t>Not what I needed, going to make my own</t>
+  </si>
+  <si>
+    <t>TRRS female connector mount</t>
+  </si>
+  <si>
+    <t>ShowMeCables</t>
+  </si>
+  <si>
+    <t>Going to make own TRRS to TRS connector</t>
   </si>
 </sst>
 </file>
@@ -236,9 +245,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="18">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -293,7 +304,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="18">
+  <cellStyles count="20">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -303,6 +314,7 @@
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -311,6 +323,7 @@
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -644,13 +657,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.6640625" bestFit="1" customWidth="1"/>
@@ -787,7 +800,7 @@
         <v>7</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -810,7 +823,7 @@
         <v>7</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -881,26 +894,23 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="1">
+      <c r="A11" s="2">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D11" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="4">
-        <v>15</v>
+        <v>6.34</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="5" customHeight="1">
@@ -1012,10 +1022,27 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="6"/>
-      <c r="F18" s="2"/>
+      <c r="A18" s="1">
+        <v>4</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+      <c r="E18" s="4">
+        <v>15</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="1"/>
@@ -1033,8 +1060,8 @@
         <v>24</v>
       </c>
       <c r="E20" s="9">
-        <f>SUM(E2:E16)</f>
-        <v>170.07999999999998</v>
+        <f>SUM(E2:E18)</f>
+        <v>185.42</v>
       </c>
       <c r="F20" s="2"/>
     </row>

</xml_diff>